<commit_message>
booking api test report update
</commit_message>
<xml_diff>
--- a/booking-api-test-report.xlsx
+++ b/booking-api-test-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadim\OneDrive\Desktop\D Drive\apache-jmeter-5.6.3\bin\SDET\assignment 3\j meter assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB784BE-FBD2-4ACA-9235-3F66857B4597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE26FC3-0378-4624-A9D6-6A02CB6CB9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load test report" sheetId="1" r:id="rId1"/>
@@ -105,13 +105,13 @@
     <t>Test 6</t>
   </si>
   <si>
-    <t>Lower bottleneck point = 3.18</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stress test successful in the expected load </t>
   </si>
   <si>
-    <t>Capacity: 3800 /1200 = 3.16</t>
+    <t>Lower bottleneck point = 3.18 TPS (0.90 % error)</t>
+  </si>
+  <si>
+    <t>Capacity = 3.16 TPS (0.81 % error)</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,11 +527,23 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1006,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0A169D-18C5-4997-B9BE-246AF9D62E59}">
   <dimension ref="D1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1236,7 @@
       <c r="H14" s="10">
         <v>3800</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="37">
         <v>8.0999999999999996E-3</v>
       </c>
     </row>
@@ -1264,7 +1276,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="31" t="s">
         <v>24</v>
       </c>
@@ -1274,25 +1286,25 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
     </row>
-    <row r="18" spans="4:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="4:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-    </row>
-    <row r="19" spans="4:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
booking test report update
</commit_message>
<xml_diff>
--- a/booking-api-test-report.xlsx
+++ b/booking-api-test-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadim\OneDrive\Desktop\D Drive\apache-jmeter-5.6.3\bin\SDET\assignment 3\j meter assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE26FC3-0378-4624-A9D6-6A02CB6CB9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F23CC4-4646-4291-8AA3-2B90C46F07DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
     <t>Lower bottleneck point = 3.18 TPS (0.90 % error)</t>
   </si>
   <si>
-    <t>Capacity = 3.16 TPS (0.81 % error)</t>
+    <t xml:space="preserve">Capacity = 2.77 TPS </t>
   </si>
 </sst>
 </file>
@@ -488,6 +488,9 @@
     <xf numFmtId="10" fontId="3" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,9 +544,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,7 +833,7 @@
   <dimension ref="D1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D12" sqref="D12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,32 +843,32 @@
   <sheetData>
     <row r="1" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="4:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="4:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
     </row>
     <row r="5" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
@@ -979,7 +979,7 @@
         <v>3333.333333333333</v>
       </c>
       <c r="I10" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>6.9999999999999999E-4</v>
       </c>
     </row>
     <row r="11" spans="4:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -990,19 +990,19 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="5">
-        <v>2.76</v>
+        <v>2.77</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="4:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1019,7 +1019,7 @@
   <dimension ref="D1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:I17"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,32 +1029,32 @@
   <sheetData>
     <row r="1" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="4:9" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
     </row>
     <row r="5" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D5" s="8" t="s">
@@ -1164,8 +1164,8 @@
         <f>G10*H7</f>
         <v>3333.333333333333</v>
       </c>
-      <c r="I10" s="12">
-        <v>2.5000000000000001E-3</v>
+      <c r="I10" s="19">
+        <v>6.9999999999999999E-4</v>
       </c>
     </row>
     <row r="11" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -1236,7 +1236,7 @@
       <c r="H14" s="10">
         <v>3800</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="12">
         <v>8.0999999999999996E-3</v>
       </c>
     </row>
@@ -1277,34 +1277,34 @@
       </c>
     </row>
     <row r="17" spans="4:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="4:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="35"/>
     </row>
     <row r="19" spans="4:9" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>